<commit_message>
Added tests to practice gherkins
</commit_message>
<xml_diff>
--- a/new_df.xlsx
+++ b/new_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,10 +478,8 @@
           <t>Remove scratches on my car</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="D3" t="n">
+        <v>250</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -503,10 +501,8 @@
           <t>Help learning and building a website</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+      <c r="D4" t="n">
+        <v>35</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -528,10 +524,8 @@
           <t>Dishwasher door</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D5" t="n">
+        <v>5</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -553,10 +547,8 @@
           <t>Professional Resume for High Profile Government Position</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="D6" t="n">
+        <v>30</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -578,10 +570,8 @@
           <t>Document Processing Platform development</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
+      <c r="D7" t="n">
+        <v>3000</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -603,10 +593,8 @@
           <t>Resume writing</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="D8" t="n">
+        <v>100</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -628,10 +616,8 @@
           <t>Help creating my new business logo</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="D9" t="n">
+        <v>100</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -653,10 +639,8 @@
           <t>Vectorworks</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+      <c r="D10" t="n">
+        <v>40</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -678,10 +662,8 @@
           <t>Leave Two x 5 star Google Reviews for my business</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D11" t="n">
+        <v>5</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -703,10 +685,8 @@
           <t>SEO work for a website</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>200</t>
-        </is>
+      <c r="D12" t="n">
+        <v>200</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -728,10 +708,8 @@
           <t>Hi there I’m needing a logo done for a beauty business</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D13" t="n">
+        <v>5</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -753,10 +731,8 @@
           <t>Need 5 website clients</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="D14" t="n">
+        <v>100</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -778,10 +754,8 @@
           <t>Hi there I’m needing a logo done for a beauty business</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D15" t="n">
+        <v>5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -803,10 +777,8 @@
           <t>Crochet clothing</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>5000</t>
-        </is>
+      <c r="D16" t="n">
+        <v>5000</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -828,10 +800,8 @@
           <t>Leave Two x 5 star Google Reviews for my business</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D17" t="n">
+        <v>5</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -853,10 +823,8 @@
           <t>Assistance with Property Management license course</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>250</t>
-        </is>
+      <c r="D18" t="n">
+        <v>250</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -878,10 +846,8 @@
           <t>Teach me how to design a website</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>30</t>
-        </is>
+      <c r="D19" t="n">
+        <v>30</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -903,10 +869,8 @@
           <t>Leave Two x 5 star Google Reviews for my business</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="D20" t="n">
+        <v>15</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -928,10 +892,8 @@
           <t>Create 2x custom photo luggage tags using sublimation printer</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D21" t="n">
+        <v>5</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -953,10 +915,8 @@
           <t>APS6 EOI assistance</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D22" t="n">
+        <v>5</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -978,10 +938,8 @@
           <t>Business Logo Design</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="D23" t="n">
+        <v>50</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1003,10 +961,8 @@
           <t>Need someone to apply for jobs on my behalf</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D24" t="n">
+        <v>5</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1028,10 +984,8 @@
           <t>Need a logo made.</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="D25" t="n">
+        <v>20</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1053,10 +1007,8 @@
           <t>Explain crypto and exchange platforms - visually preferred</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="D26" t="n">
+        <v>20</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1078,10 +1030,8 @@
           <t>Build 5 page website</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>350</t>
-        </is>
+      <c r="D27" t="n">
+        <v>350</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1103,10 +1053,8 @@
           <t>Written Report</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>50</t>
-        </is>
+      <c r="D28" t="n">
+        <v>50</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1128,10 +1076,8 @@
           <t>Preparing for job interview finance role</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
+      <c r="D29" t="n">
+        <v>25</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1153,10 +1099,8 @@
           <t>Leave Two x 5 star Google Reviews for my business</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="D30" t="n">
+        <v>5</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1178,10 +1122,8 @@
           <t>Gardon edging</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>500</t>
-        </is>
+      <c r="D31" t="n">
+        <v>500</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1203,14 +1145,2142 @@
           <t>SEO Expert Required For Audit</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="D32" t="n">
+        <v>50</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Chelsee</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/builder-renovation-x01htmhf5k97ns083jzbvw58g3b/</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Builder/renovation</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/administration-x01htmhbma6141ykwmde8ahbfej/</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>30</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Gauri</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmha93t7r1t1273kxsw29vn/</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>11</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/graphic-design-for-trade-van-x01htmh74zzyfcyrytkagb9p5e2/</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>11</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/selection-criteria-responses-x01htmgrzp520f93kc8gvse2rjb/</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Selection criteria application letter needed asap</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>20</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Terina</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/need-account-declartion-form-x01hth549s1gjvdxv66gq6ybf31/</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Accountant Declaration form signning</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>25</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/door-720x2040install-only-x01htmgga6q1dvkjxc3bbn92k8m/</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Door 720x2040install only.</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>50</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Wade</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-a-home-office-for-a-1-2-day-film-shoot-x01htmgce556g8wct254j6jz278/</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>I need to hire a home office for a 1/2 day film shoot</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>800</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-a-location-for-a-1-2-day-film-shoot-front-of-mansion-x01htmenhrn5hqyb1aapv4cqf5x/</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>I need to hire a location for a 1/2 day film shoot: front of mansion</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>800</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-location-car-mechanic-for-1-2-day-film-shoot-x01htmfvc7dmh15d8vga3ryc4vk/</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>I need to hire location (car mechanic) for 1/2 day film shoot</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>900</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/5-myositis-patients-to-review-questionnaire-x01htmg0x6yewcks5ge1s7xqh3d/</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>5 - MYOSITIS PATIENTS TO REVIEW QUESTIONNAIRE</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>75</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Kym</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/google-adwords-x01htmfn0d0nyjhjakr72vk718s/</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Google Adwords</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/send-1-item-with-any-vehicle-from-brunswick-east-to-wilson-6107-wa-x01htmehbxaz6yj8t5z2awagb7e/</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Send 1 item with any vehicle from Brunswick East to Wilson 6107 Perth</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>120</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Jason</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/make-a-tony-cart-in-beam-ng-x01htmeszhx44bx6fz2v4m22mz1/</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Make a tony cart in beam ng</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>50</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Wendy</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/obesity-diabetes-patients-to-review-questionnaires-x01hrv0zr55endnmrjngse5v45k/</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Make a tony cart in beam ng</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>50</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Kym</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmehq350d290vaah6kwrymh/</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>11</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/website-design-i-want-someone-to-design-website-on-shopify-x01htmbaf52q5xqy2pytrcad70j/</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>11</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/draft-a-retaining-wall-for-a-1-8-terraced-wall-x01htmchaybmyfqeqbg8a214z00/</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Draft a retaining wall for a 1.8 (terraced) wall.</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>350</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/selection-criteria-cover-letter-and-resume-x01htmbxjaf2bpegst99vzjff3b/</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>selection criteria, cover letter and resume</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>80</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Shrawan</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/social-media-marketing-x01htmbwm4f68efacj7b1fn44sm/</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Social media marketing</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>50</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Mayur</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/website-remade-x01htmb0azbgwtv77pfxk7syv4d/</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Social media marketing</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>50</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Mayur</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/repaint-reseal-pergola-concrete-x01htma6k3fzxtbz0w0m00xstcr/</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Repaint &amp; Reseal pergola concrete</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Darren</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/build-instagram-account-x01htm5nwh0cfcgvfpmx5v9p2md/</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Build Instagram account</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>120</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Juliet</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sugar-chemist-trainee-application-x01htm9vf6rgfge46d1k11mxkev/</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Sugar chemist trainee application</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>50</v>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>Nikki</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/photo-editing-x01htm96ncmmmcfavre35mmw8n1/</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Photo editing</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>32</v>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>Aleisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/professional-video-editor-x01htm94hec7bj6e7emkf1cdzwv/</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Professional video editor</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>5</v>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>Mohan</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/build-app-using-bubble-x01htm8sa32evhty8c9q0ema50f/</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Build app using bubble</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>500</v>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>Salem</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/assistance-and-advice-on-disability-discrimination-x01htm85v66dhhp54mm4830rx5x/</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Assistance and advice on disability discrimination</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>100</v>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>Kristen</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/a-bookkeeper-resume-needed-x01htm8gqc835vwy4695c9bfqz3/</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>A bookkeeper resume and cover letter needed</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>20</v>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Tessa</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/set-up-etsy-digital-product-store-x01htm8eq8ye07w339xj9qbq70f/</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Set up Etsy digital product store</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>5</v>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Maryjean</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/2x-car-roadworthys-x01htmmzc4kbha7w5gsm1m80txn/</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>2x car roadworthys</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>300</v>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>Lachlan</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/furniture-carpenters-x01htmmnaq0fxwvdqa1ccjws996/</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Furniture carpenters</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>300</v>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Tania</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/logo-menu-slides-x01htmmmxtqg685914b8x6d3v4v/</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Logo, menu,slides</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>100</v>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/assistance-and-advice-on-disability-discrimination-x01htm85v66dhhp54mm4830rx5x/</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Assistance and advice on disability discrimination</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>200</v>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Kristen</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/testing-by-signing-up-a-new-app-new-user-only-x01htmm4fet76d7t4m0g0pa5h6z/</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Testing by Signing up a New app (New user only)</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>5</v>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>LiLi</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/quote-panel-bent-x01htmm1bvjr5znpeedjcwd100c/</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Quote panel bent</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>100</v>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Edward</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/photo-editing-x01htmj7xx1hwa54t2mxzns9b15/</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Photo editing</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>20</v>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Aleisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/draw-something-x01htmj43tr3eppvcdkd7v35rba/</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Draw something</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>7</v>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Raphael</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmhsvr70kcx5x7zfxj66kmm/</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>8</v>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmhrxveyamwtgac7nfry9r1/</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>11</v>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/want-to-edit-2-photos-x01htmhpqkeshhpzdtxhj2qa58z/</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Want to edit 2 photos</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>20</v>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>Aliezay</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/door-720x2040install-only-x01htmgga6q1dvkjxc3bbn92k8m/</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Door 720x2040install only.</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>50</v>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>Wade</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/builder-renovation-x01htmhf5k97ns083jzbvw58g3b/</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Builder/renovation</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>Mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/administration-x01htmhbma6141ykwmde8ahbfej/</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>30</v>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Gauri</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmha93t7r1t1273kxsw29vn/</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>11</v>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/graphic-design-for-trade-van-x01htmh74zzyfcyrytkagb9p5e2/</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Graphic design for trade van</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>150</v>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>William</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/selection-criteria-responses-x01htmgrzp520f93kc8gvse2rjb/</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Selection criteria application letter needed asap</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>20</v>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Terina</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/need-account-declartion-form-x01hth549s1gjvdxv66gq6ybf31/</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Accountant Declaration form signning</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>25</v>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-a-home-office-for-a-1-2-day-film-shoot-x01htmgce556g8wct254j6jz278/</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>I need to hire a home office for a 1/2 day film shoot</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>800</v>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-a-location-for-a-1-2-day-film-shoot-front-of-mansion-x01htmenhrn5hqyb1aapv4cqf5x/</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>I need to hire a location for a 1/2 day film shoot: front of mansion</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>800</v>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-location-car-mechanic-for-1-2-day-film-shoot-x01htmfvc7dmh15d8vga3ryc4vk/</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>I need to hire location (car mechanic) for 1/2 day film shoot</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>900</v>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/5-myositis-patients-to-review-questionnaire-x01htmg0x6yewcks5ge1s7xqh3d/</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>5 - MYOSITIS PATIENTS TO REVIEW QUESTIONNAIRE</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>75</v>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>Kym</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/google-adwords-x01htmfn0d0nyjhjakr72vk718s/</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Google Adwords</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/send-1-item-with-any-vehicle-from-brunswick-east-to-wilson-6107-wa-x01htmehbxaz6yj8t5z2awagb7e/</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Send 1 item with any vehicle from Brunswick East to Wilson 6107 Perth</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>120</v>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Jason</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/make-a-tony-cart-in-beam-ng-x01htmeszhx44bx6fz2v4m22mz1/</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Make a tony cart in beam ng</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>50</v>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>Wendy</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/obesity-diabetes-patients-to-review-questionnaires-x01hrv0zr55endnmrjngse5v45k/</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Make a tony cart in beam ng</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>50</v>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>Wendy</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmehq350d290vaah6kwrymh/</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>11</v>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/website-design-i-want-someone-to-design-website-on-shopify-x01htmbaf52q5xqy2pytrcad70j/</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>11</v>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/draft-a-retaining-wall-for-a-1-8-terraced-wall-x01htmchaybmyfqeqbg8a214z00/</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Draft a retaining wall for a 1.8 (terraced) wall.</t>
+        </is>
+      </c>
+      <c r="D91" t="n">
+        <v>350</v>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/selection-criteria-cover-letter-and-resume-x01htmbxjaf2bpegst99vzjff3b/</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>selection criteria, cover letter and resume</t>
+        </is>
+      </c>
+      <c r="D92" t="n">
+        <v>80</v>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>Shrawan</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/power-bi-report-build-from-d365-data-source-x01htmrha2v2mqvsyv7s01t7mqq/</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Power Bi report build from D365 data source</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>Vijay</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/worden-certificate-frame-x01htmqk164ns6y4vfb7nxrcasj/</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Worden certificate frame</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>H</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/screenshots-transposed-into-screenplay-docx-format-x01htmqbpgff0604g35y8s16ab6/</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Screenshots transposed into screenplay .docx format</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/looking-for-a-unicorn-va-with-marketing-experience-c-x01htmq53g5xnnghwwpwdatvn84/</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Looking for a unicorn VA with marketing experience 🦄</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Amy</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/correct-my-resume-and-create-cover-letter-x01htmpkrfsb3r4j226vhd3b61k/</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Correct my resume and create cover letter</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>Nabil</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/setup-devops-on-azure-local-server-x01htmnxst2r17sy9cyb208w2yz/</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Setup DevOps on Azure &amp; Local Server</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>Lenard</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/2x-car-roadworthys-x01htmmzc4kbha7w5gsm1m80txn/</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>2x car roadworthys</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Lachlan</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/furniture-carpenters-x01htmmnaq0fxwvdqa1ccjws996/</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Furniture carpenters</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>300</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>Tania</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/logo-menu-slides-x01htmmmxtqg685914b8x6d3v4v/</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Logo, menu,slides</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/assistance-and-advice-on-disability-discrimination-x01htm85v66dhhp54mm4830rx5x/</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Assistance and advice on disability discrimination</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>Kristen</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/testing-by-signing-up-a-new-app-new-user-only-x01htmm4fet76d7t4m0g0pa5h6z/</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Testing by Signing up a New app (New user only)</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>LiLi</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/quote-panel-bent-x01htmm1bvjr5znpeedjcwd100c/</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Quote panel bent</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>Edward</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/photo-editing-x01htmj7xx1hwa54t2mxzns9b15/</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Photo editing</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>Aleisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/draw-something-x01htmj43tr3eppvcdkd7v35rba/</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Draw something</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>Raphael</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmhsvr70kcx5x7zfxj66kmm/</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmhrxveyamwtgac7nfry9r1/</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/want-to-edit-2-photos-x01htmhpqkeshhpzdtxhj2qa58z/</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Want to edit 2 photos</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Aliezay</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/door-720x2040install-only-x01htmgga6q1dvkjxc3bbn92k8m/</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Door 720x2040install only.</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
         <is>
           <t>50</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Chelsee</t>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Wade</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/builder-renovation-x01htmhf5k97ns083jzbvw58g3b/</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Builder/renovation</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>Mo</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/administration-x01htmhbma6141ykwmde8ahbfej/</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Administration</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Gauri</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/sign-up-to-an-app-x01htmha93t7r1t1273kxsw29vn/</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/graphic-design-for-trade-van-x01htmh74zzyfcyrytkagb9p5e2/</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Sign up to an app</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Benjamin</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/selection-criteria-responses-x01htmgrzp520f93kc8gvse2rjb/</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Selection criteria application letter needed asap</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Terina</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/need-account-declartion-form-x01hth549s1gjvdxv66gq6ybf31/</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Accountant Declaration form signning</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Anthony</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-a-home-office-for-a-1-2-day-film-shoot-x01htmgce556g8wct254j6jz278/</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>I need to hire a home office for a 1/2 day film shoot</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-a-location-for-a-1-2-day-film-shoot-front-of-mansion-x01htmenhrn5hqyb1aapv4cqf5x/</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>I need to hire a location for a 1/2 day film shoot: front of mansion</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/i-need-to-hire-location-car-mechanic-for-1-2-day-film-shoot-x01htmfvc7dmh15d8vga3ryc4vk/</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>I need to hire location (car mechanic) for 1/2 day film shoot</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Heidi</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/5-myositis-patients-to-review-questionnaire-x01htmg0x6yewcks5ge1s7xqh3d/</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>5 - MYOSITIS PATIENTS TO REVIEW QUESTIONNAIRE</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Kym</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/google-adwords-x01htmfn0d0nyjhjakr72vk718s/</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>Google Adwords</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>https://www.airtasker.com/tasks/send-1-item-with-any-vehicle-from-brunswick-east-to-wilson-6107-wa-x01htmehbxaz6yj8t5z2awagb7e/</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>Send 1 item with any vehicle from Brunswick East to Wilson 6107 Perth</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Jason</t>
         </is>
       </c>
     </row>

</xml_diff>